<commit_message>
NO BUILD dev updates to game
</commit_message>
<xml_diff>
--- a/Assignment2/B4 Self and Peer Assessment Documentation/New Self and Peer Assessment Spreadsheet.xlsx
+++ b/Assignment2/B4 Self and Peer Assessment Documentation/New Self and Peer Assessment Spreadsheet.xlsx
@@ -531,7 +531,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -684,28 +684,10 @@
       <c r="M8" s="6"/>
       <c r="N8" s="7"/>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D9" s="0"/>
-    </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="C10" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="D10" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="E10" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="F10" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="G10" s="1" t="n">
-        <v>23</v>
-      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="G10" s="1"/>
       <c r="K10" s="22" t="s">
         <v>13</v>
       </c>

</xml_diff>